<commit_message>
Processed data batch by batch within tasks.
</commit_message>
<xml_diff>
--- a/TSR Data Analysis.xlsx
+++ b/TSR Data Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sources\personal\remote\File-Downloader\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71A1BFDA-D9F2-4314-B396-89F993464458}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A133D2D-4663-49D3-8245-671501282799}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2781052E-7190-4080-9D53-E268C290EA6B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="25">
   <si>
     <t xml:space="preserve">API Version </t>
   </si>
@@ -102,13 +102,22 @@
   </si>
   <si>
     <t>426?</t>
+  </si>
+  <si>
+    <t>DB call - async, with CF and ToListAsync()</t>
+  </si>
+  <si>
+    <t>404?</t>
+  </si>
+  <si>
+    <t>171/135</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,6 +129,21 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -163,7 +187,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -178,6 +202,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -495,16 +531,16 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEB4489D-F2E1-4D14-8980-4033DE5C9C21}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="30.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.5546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="36.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.33203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="14" style="1" customWidth="1"/>
     <col min="5" max="5" width="13.21875" style="1" customWidth="1"/>
@@ -585,7 +621,7 @@
         <v>2000000</v>
       </c>
       <c r="E3" s="1">
-        <f t="shared" ref="E3:E20" si="0">C3*D3</f>
+        <f t="shared" ref="E3:E25" si="0">C3*D3</f>
         <v>4000000</v>
       </c>
       <c r="F3" s="1">
@@ -655,30 +691,30 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B6" s="1" t="s">
+    <row r="6" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="8">
         <v>10</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="8">
         <v>400000</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="8">
         <f t="shared" si="0"/>
         <v>4000000</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="8">
         <v>60</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="8">
         <v>181</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6" s="8">
         <v>254</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="I6" s="8" t="s">
         <v>8</v>
       </c>
     </row>
@@ -709,35 +745,35 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B8" s="1" t="s">
+    <row r="8" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="8">
         <v>40</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="8">
         <v>100000</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="8">
         <f t="shared" si="0"/>
         <v>4000000</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="8">
         <v>58</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8" s="8">
         <v>151</v>
       </c>
-      <c r="H8" s="1">
+      <c r="H8" s="8">
         <v>221</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="I8" s="8" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
@@ -745,201 +781,320 @@
         <v>13</v>
       </c>
       <c r="C10" s="1">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1">
+        <v>4000000</v>
+      </c>
+      <c r="E10" s="1">
+        <f>C10*D10</f>
+        <v>4000000</v>
+      </c>
+      <c r="F10" s="1">
+        <v>135</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="8">
         <v>10</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D11" s="8">
         <v>400000</v>
       </c>
-      <c r="E10" s="1">
-        <f t="shared" ref="E10:E15" si="1">C10*D10</f>
-        <v>4000000</v>
-      </c>
-      <c r="F10" s="1">
-        <v>70</v>
-      </c>
-      <c r="G10" s="4" t="s">
+      <c r="E11" s="8">
+        <f t="shared" ref="E11:E12" si="1">C11*D11</f>
+        <v>4000000</v>
+      </c>
+      <c r="F11" s="8">
+        <v>52</v>
+      </c>
+      <c r="G11" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="I10" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C11" s="1">
+      <c r="I11" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="1">
         <v>20</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D12" s="1">
         <v>200000</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E12" s="1">
         <f t="shared" si="1"/>
         <v>4000000</v>
       </c>
-      <c r="F11" s="1">
-        <v>54</v>
-      </c>
-      <c r="G11" s="4" t="s">
+      <c r="F12" s="1">
+        <v>68</v>
+      </c>
+      <c r="G12" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I11" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C12" s="1">
+      <c r="I12" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="8">
         <v>40</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D13" s="8">
         <v>100000</v>
       </c>
-      <c r="E12" s="1">
-        <f>C12*D12</f>
-        <v>4000000</v>
-      </c>
-      <c r="F12" s="1">
+      <c r="E13" s="8">
+        <f>C13*D13</f>
+        <v>4000000</v>
+      </c>
+      <c r="F13" s="8">
         <v>56</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="G13" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="I12" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="G13" s="4"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="G14" s="4"/>
-    </row>
-    <row r="16" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
+      <c r="I13" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1</v>
+      </c>
+      <c r="D15" s="1">
+        <v>4000000</v>
+      </c>
+      <c r="E15" s="1">
+        <f>C15*D15</f>
+        <v>4000000</v>
+      </c>
+      <c r="F15" s="1">
+        <v>247</v>
+      </c>
+      <c r="G15" s="7">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="1">
+        <v>10</v>
+      </c>
+      <c r="D16" s="1">
+        <v>400000</v>
+      </c>
+      <c r="E16" s="1">
+        <f t="shared" ref="E16:E17" si="2">C16*D16</f>
+        <v>4000000</v>
+      </c>
+      <c r="F16" s="1">
+        <v>121</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
+      <c r="B17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="1">
+        <v>20</v>
+      </c>
+      <c r="D17" s="1">
+        <v>200000</v>
+      </c>
+      <c r="E17" s="1">
+        <f t="shared" si="2"/>
+        <v>4000000</v>
+      </c>
+      <c r="F17" s="1">
+        <v>124</v>
+      </c>
+      <c r="G17" s="4"/>
+      <c r="I17" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="1">
+        <v>40</v>
+      </c>
+      <c r="D18" s="1">
+        <v>100000</v>
+      </c>
+      <c r="E18" s="1">
+        <f>C18*D18</f>
+        <v>4000000</v>
+      </c>
+      <c r="F18" s="1">
+        <v>123</v>
+      </c>
+      <c r="G18" s="4"/>
+      <c r="I18" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G19" s="4"/>
+    </row>
+    <row r="21" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C22" s="1">
         <v>1</v>
       </c>
-      <c r="D17" s="1">
-        <v>4000000</v>
-      </c>
-      <c r="E17" s="1">
+      <c r="D22" s="1">
+        <v>4000000</v>
+      </c>
+      <c r="E22" s="1">
         <f t="shared" si="0"/>
         <v>4000000</v>
       </c>
-      <c r="F17" s="1">
+      <c r="F22" s="1">
         <v>548</v>
       </c>
-      <c r="G17" s="1">
+      <c r="G22" s="1">
         <v>143</v>
       </c>
-      <c r="H17" s="1">
+      <c r="H22" s="1">
         <v>714</v>
       </c>
-      <c r="I17" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="1">
+      <c r="I22" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+      <c r="C23" s="1">
         <v>1</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D23" s="1">
         <v>2000000</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E23" s="1">
         <f t="shared" si="0"/>
         <v>2000000</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F23" s="1">
         <v>41</v>
       </c>
-      <c r="G18" s="1">
+      <c r="G23" s="1">
         <v>35</v>
       </c>
-      <c r="H18" s="1">
+      <c r="H23" s="1">
         <v>91</v>
       </c>
-      <c r="I18" s="1" t="s">
+      <c r="I23" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
-      <c r="C19" s="1">
+    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+      <c r="C24" s="1">
         <v>1</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D24" s="1">
         <v>1000000</v>
       </c>
-      <c r="E19" s="1">
+      <c r="E24" s="1">
         <f t="shared" si="0"/>
         <v>1000000</v>
       </c>
-      <c r="F19" s="1">
+      <c r="F24" s="1">
         <v>17</v>
       </c>
-      <c r="G19" s="1">
+      <c r="G24" s="1">
         <v>10</v>
       </c>
-      <c r="H19" s="1">
+      <c r="H24" s="1">
         <v>30</v>
       </c>
-      <c r="I19" s="1" t="s">
+      <c r="I24" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
-      <c r="C20" s="1">
+    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+      <c r="C25" s="1">
         <v>1</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D25" s="1">
         <v>500000</v>
       </c>
-      <c r="E20" s="1">
+      <c r="E25" s="1">
         <f t="shared" si="0"/>
         <v>500000</v>
       </c>
-      <c r="F20" s="1">
+      <c r="F25" s="1">
         <v>9</v>
       </c>
-      <c r="G20" s="1">
+      <c r="G25" s="1">
         <v>4</v>
       </c>
-      <c r="H20" s="1">
+      <c r="H25" s="1">
         <v>13</v>
       </c>
-      <c r="I20" s="1" t="s">
+      <c r="I25" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
+    <row r="26" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B27" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C27" s="1">
         <v>1</v>
       </c>
-      <c r="D22" s="1">
-        <v>4000000</v>
-      </c>
-      <c r="E22" s="1">
-        <f t="shared" ref="E22" si="2">C22*D22</f>
-        <v>4000000</v>
-      </c>
-      <c r="F22" s="1">
-        <v>171</v>
-      </c>
-      <c r="G22" s="1">
+      <c r="D27" s="1">
+        <v>4000000</v>
+      </c>
+      <c r="E27" s="1">
+        <f t="shared" ref="E27" si="3">C27*D27</f>
+        <v>4000000</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G27" s="1">
         <v>59</v>
       </c>
-      <c r="I22" s="1" t="s">
+      <c r="I27" s="1" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>